<commit_message>
QC for Case 12
</commit_message>
<xml_diff>
--- a/Matching arterycodes to TCL/issues and manual corrections.xlsx
+++ b/Matching arterycodes to TCL/issues and manual corrections.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13770" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="case 2 - h-dist" sheetId="2" r:id="rId1"/>
-    <sheet name="case 3+4 - tcs" sheetId="3" r:id="rId2"/>
-    <sheet name="case 3+4 - intersections" sheetId="4" r:id="rId3"/>
-    <sheet name="case 5" sheetId="1" r:id="rId4"/>
+    <sheet name="case 12" sheetId="6" r:id="rId2"/>
+    <sheet name="case 3+4 - tcs" sheetId="3" r:id="rId3"/>
+    <sheet name="case 3+4 - intersections" sheetId="4" r:id="rId4"/>
+    <sheet name="case 5" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'case 2 - h-dist'!$F$1:$F$201</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1765" uniqueCount="805">
   <si>
     <t>Arterycode</t>
   </si>
@@ -1995,6 +1996,457 @@
   </si>
   <si>
     <t>wrong desc: geometry on lake shore blvd</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(302047.732230423 4841055.38707466,302096.769986413 4841051.33671508)</t>
+  </si>
+  <si>
+    <t>KNOB HILL DR E/B W OF CROSSROADS PL</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(326540.058074586 4846357.40777511,326722.970141714 4846412.36265387)</t>
+  </si>
+  <si>
+    <t>LAWRENCE AVE E/B W OF CEDARBRAE MALL E TCS</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(326722.970141714 4846412.36265387,326540.058074586 4846357.40777511)</t>
+  </si>
+  <si>
+    <t>LAWRENCE AVE W/B E OF CEDARBRAE MALL W TCS</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(311714.125628871 4832144.9960319,311750.955499434 4832184.87957267)</t>
+  </si>
+  <si>
+    <t>REMEMBRANCE DR N/B S OF LAKE SHORE BLVD( ONT PLACE EXITS)</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(322644.175394753 4840448.39318722,322856.980284035 4840543.39162095)</t>
+  </si>
+  <si>
+    <t>BELL ESTATE RD E/B W OF ETHEL BELL TER E LEG</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(322856.980284035 4840543.39162095,322644.175394753 4840448.39318722)</t>
+  </si>
+  <si>
+    <t>BELL ESTATE RD W/B E OF WARDEN AVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OVERLEA BLVD E/B W OF EAST YORK TOWN CENTRE E_x000D_
+</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(300793.281268487 4842856.4969728,301032.861019997 4843081.33693354)</t>
+  </si>
+  <si>
+    <t>TANDRIDGE CRES N/B N OF ARCOT BLVD</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(303511.820630286 4831270.1183624,303552.428346474 4831282.02941983)</t>
+  </si>
+  <si>
+    <t>THE QUEENSWAY E/B W OF THEATRE ENT</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(306815.620866897 4832468.11471759,307024.532430556 4832512.1586277)</t>
+  </si>
+  <si>
+    <t>THE QUEENSWAY E/B TO F G GARDINER EXPY E/B</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(315459.612109383 4851572.01071482,315829.972957818 4851249.59209128)</t>
+  </si>
+  <si>
+    <t>FRANCINE DR E/B E OF MARISA CRT</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(315829.972957818 4851249.59209128,315459.612109383 4851572.01071482)</t>
+  </si>
+  <si>
+    <t>FRANCINE DR W/B E OF MARISA CRT</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(320459.846500394 4852787.19859623,320467.088745938 4852740.06441178)</t>
+  </si>
+  <si>
+    <t>SHEPTON WAY S/B N OF WEST HIGHTLAND CREEK</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(303885.736612924 4847932.29758998,303861.865247771 4847853.9706363)</t>
+  </si>
+  <si>
+    <t>IAN MACDONALD BLVD S/B N OF SHOREHAM DR</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(303907.372615272 4847861.02126224,303885.736612924 4847932.29758998)</t>
+  </si>
+  <si>
+    <t>IAN MACDONALD LANE N/B N OF ARBORETUM LANE</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(294407.31165577 4843530.50680974,294506.376996298 4843425.49748727)</t>
+  </si>
+  <si>
+    <t>FINCH AVE E/B TO HIGHWAY 427 S/B</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(331944.686918947 4847659.00332758,331914.373419659 4847449.00468442)</t>
+  </si>
+  <si>
+    <t>RAVENVIEW DR S/B S OF DUNSTALL CRES</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(331914.373419659 4847449.00468442,331944.686918947 4847659.00332758)</t>
+  </si>
+  <si>
+    <t>RAVENVIEW DR N/B S OF DUNSTALL CRES</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(306600.25067196 4831414.19115283,306429.431010262 4831175.70998105)</t>
+  </si>
+  <si>
+    <t>MARINE PARADE DR W/B E OF PARK LAWN RD</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(299950.186554024 4846034.75913115,299464.692148295 4846516.5819062)</t>
+  </si>
+  <si>
+    <t>MILVAN DR N/B S OF MILLWICK DR</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(327334.247010199 4852932.00145148,326959.695887577 4852817.50128643)</t>
+  </si>
+  <si>
+    <t>FINCH AVE E W/B E OF BLACKBIRD GT</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(294844.230225498 4843668.80908788,294513.025344713 4843856.9457902)</t>
+  </si>
+  <si>
+    <t>FINCH AVE W/B TO HIGHWAY 427 N/B</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(310854.517274796 4837819.36978895,310722.688609324 4837788.42704193)</t>
+  </si>
+  <si>
+    <t>LN N OF ST CLAIR AVE W/B E OF HUMEWOOD DR</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(310722.688609324 4837788.42704193,310854.517274796 4837819.36978895)</t>
+  </si>
+  <si>
+    <t>LN N OF ST CLAIR AVE E/B E OF HUMEWOOD DR</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(317999.487418239 4846267.70981194,317999.487418239 4846267.70981194)</t>
+  </si>
+  <si>
+    <t>RAMP YORK MILLS RD W/B TO DON VALLEY PKWY S/B</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(323893.62772252 4846978.99295792,324072.687706881 4846799.99706711)</t>
+  </si>
+  <si>
+    <t>APPLEFIELD DR S/B S OF WATERFIELD DR</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(317737.570535826 4839410.56105102,317973.248713142 4839531.15175677)</t>
+  </si>
+  <si>
+    <t>FOUR OAKS GT N/B N OF DUNSTAN CR</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(317973.248713142 4839531.15175677,317737.570535826 4839410.56105102)</t>
+  </si>
+  <si>
+    <t>FOUR OAKS GT S/B N OF DUNSTAN CR</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(317145.323121179 4843850.72523795,317014.228578547 4843625.45523903)</t>
+  </si>
+  <si>
+    <t>THE DONWAY W S/B N OF SANDERLING PL</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(317014.228578547 4843625.45523903,317145.323121179 4843850.72523795)</t>
+  </si>
+  <si>
+    <t>THE DONWAY WEST N/B S OF LAWRENCE AVE</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(306734.826111653 4831874.15198703,306600.25067196 4831414.19115283)</t>
+  </si>
+  <si>
+    <t>MARINE PARADE DR S/B N OF HUMBER BAY PARK</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(315181.123847359 4838357.00751911,315049.748853305 4838171.5010503)</t>
+  </si>
+  <si>
+    <t>DOUGLAS DR S/B S OF GLEN RD</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(315049.748853305 4838171.5010503,315181.123847359 4838357.00751911)</t>
+  </si>
+  <si>
+    <t>DOUGLAS DR N/B S OF GLEN RD</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(312246.801862062 4839404.23048901,312054.973089429 4839654.92274486)</t>
+  </si>
+  <si>
+    <t>FOREST HILL RD N/B N OF HILHOLM RD</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(312054.973089429 4839654.92274486,312246.801862062 4839404.23048901)</t>
+  </si>
+  <si>
+    <t>FOREST HILL RD S/B N OF HILHOLM RD</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(294394.938798918 4843547.49831821,294351.097642806 4843531.95693848)</t>
+  </si>
+  <si>
+    <t>FINCH AVE W/B E OF LONGO CIR</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(294351.097642806 4843531.95693848,294394.938798918 4843547.49831821)</t>
+  </si>
+  <si>
+    <t>FINCH AVE E/B E OF LONGO CIR</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(308274.306452602 4845274.98167996,308078.353394351 4845342.64768719)</t>
+  </si>
+  <si>
+    <t>FINDLAY BLVD N/B N OF EMBRO DR</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(308078.353394351 4845342.64768719,308274.306452602 4845274.98167996)</t>
+  </si>
+  <si>
+    <t>FINDLAY BLVD S/B N OF EMBRO DR</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(317830.457696499 4846215.09514094,318057.829562582 4846023.49813143)</t>
+  </si>
+  <si>
+    <t>RAMP YORK MILLS RD E/B &amp; W/B TO DON VALLEY PKWY S/B</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(310931.270230134 4844354.14993077,311077.682369549 4844273.37275957)</t>
+  </si>
+  <si>
+    <t>HIGHWAY 401 E/B TO AVENUE RD S/B</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(299621.349013183 4831671.79402218,299638.728752775 4831678.49461705)</t>
+  </si>
+  <si>
+    <t>DUNDAS ST E/B W OF ETOBICOKE CREEK BRIDGE</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(318623.02166358 4840051.25793053,318846.632181179 4840208.23186629)</t>
+  </si>
+  <si>
+    <t>ALDER RD N/B S OF PARKVIEW HILL CR</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(318846.632181179 4840208.23186629,318623.02166358 4840051.25793053)</t>
+  </si>
+  <si>
+    <t>ALDER RD S/B S OF PARKVIEW HILL CR</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(297911.428444814 4840787.03325086,298478.385740055 4840624.88885608)</t>
+  </si>
+  <si>
+    <t>BETHRIDGE RD E/B W OF MARTIN GROVE RD</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(309603.753424202 4846914.00718865,309567.006039352 4846903.89629102)</t>
+  </si>
+  <si>
+    <t>BETTY ANN DR W/B E OF BATHURST ST</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(310854.517274796 4837819.36978895,310962.928246533 4837850.80257947)</t>
+  </si>
+  <si>
+    <t>LN N OF ST CLAIR AVE E/B E  OF PINEWOOD AVE</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(310962.928246533 4837850.80257947,310854.517274796 4837819.36978895)</t>
+  </si>
+  <si>
+    <t>LN N OF ST CLAIR AVE W/B W OF PINEWOOD AVE</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(319981.561345925 4848464.00479365,320188.311783921 4848324.5524134)</t>
+  </si>
+  <si>
+    <t>PALMDALE DR SB S OF SHEPPARD AVE</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(320188.311783921 4848324.5524134,319981.561345925 4848464.00479365)</t>
+  </si>
+  <si>
+    <t>PALMDALE DR NB S OF SHEPPARD AVE</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(314414.188191105 4833221.18157303,314414.188191105 4833221.18157303)</t>
+  </si>
+  <si>
+    <t>RAMP F G GARDINER EXPY E/B TO YORK ST</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(301106.908443971 4842153.00451845,301254.252671935 4842026.00324359)</t>
+  </si>
+  <si>
+    <t>ALBION RD E/B E OF ARMEL CRT</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(301254.252671935 4842026.00324359,301106.908443971 4842153.00451845)</t>
+  </si>
+  <si>
+    <t>ALBION RD W/B E OF ARMEL CRT</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(307424.20870116 4845552.61632769,307732.680519621 4845366.83983491)</t>
+  </si>
+  <si>
+    <t>SHEPPARD AVE E/B W OF W R ALLEN RD</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(307732.680519621 4845366.83983491,307424.20870116 4845552.61632769)</t>
+  </si>
+  <si>
+    <t>SHEPPARD AVE W/B E OF KODIAK CR</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(308585.558039569 4844620.15354592,308478.235879236 4844443.48786197)</t>
+  </si>
+  <si>
+    <t>WILSON HEIGHTS S/B TO W R ALLEN RD SB &amp; NB</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(312847.998976498 4838223.42566004,312778.570752417 4838124.85690935)</t>
+  </si>
+  <si>
+    <t>FOXBAR RD S/B N OF AVENUE RD</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(327749.669803289 4853599.5307131,327736.719546451 4853700.07963958)</t>
+  </si>
+  <si>
+    <t>KNOWLES DR S/B N OF OSPREY CRT</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(327736.719546451 4853700.07963958,327749.669803289 4853599.5307131)</t>
+  </si>
+  <si>
+    <t>KNOWLES DR N/B N OF OSPREY CRT</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(319349.374349359 4846108.12564445,319343.204418076 4846248.4781046)</t>
+  </si>
+  <si>
+    <t>COMBERMERE DR W/B E OF PARKWOOD VILLAGE DR</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(319343.204418076 4846248.4781046,319349.374349359 4846108.12564445)</t>
+  </si>
+  <si>
+    <t>COMBERMERE DR E/B W OF CANNONBURY CRT</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(327495.374600697 4853135.6995353,327704.187181502 4853017.3690302)</t>
+  </si>
+  <si>
+    <t>FINCH AVE S/B N OF OLD FINCH AVE</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(327704.187181502 4853017.3690302,327495.374600697 4853135.6995353)</t>
+  </si>
+  <si>
+    <t>MORNINGSIDE AVE N/B N OF OLD FINCH AVE</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(305527.276525758 4843935.38275364,305833.166541424 4843852.52539777)</t>
+  </si>
+  <si>
+    <t>WHITBURN CRES E/B W OF BLAYDON AV</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(305833.166541424 4843852.52539777,305527.276525758 4843935.38275364)</t>
+  </si>
+  <si>
+    <t>WHITBURN CRES W/B E OF SKIPTON CRT</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(319798.063630239 4836018.57991922,319897.590890756 4836161.49260666)</t>
+  </si>
+  <si>
+    <t>EASTERN AVE N/B S OF QUEEN ST</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(319897.590890756 4836161.49260666,319798.063630239 4836018.57991922)</t>
+  </si>
+  <si>
+    <t>EASTERN AVE S/B S OF QUEEN ST</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(309571.616990672 4840861.71988136,309700.624644782 4841005.54264959)</t>
+  </si>
+  <si>
+    <t>GLEN PARK AVE N/B N OF GLENCAIRN AVE</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(309700.624644782 4841005.54264959,309571.616990672 4840861.71988136)</t>
+  </si>
+  <si>
+    <t>GLEN PARK AVE S/B N OF GLENCAIRN AVE</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(311758.890624962 4849454.62273829,311626.92998235 4849317.77058889)</t>
+  </si>
+  <si>
+    <t>AVERILL CRES S/B N OF MULLET RD</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(311626.92998235 4849317.77058889,311758.890624962 4849454.62273829)</t>
+  </si>
+  <si>
+    <t>AVERILL CRES N/B S OF SILVERVIEW DR</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(302300.484950194 4842637.22750659,302141.172045369 4842712.58419657)</t>
+  </si>
+  <si>
+    <t>ROCKBANK CRES N/B S OF STARVIEW DR</t>
+  </si>
+  <si>
+    <t>SRID=82181;LINESTRING(302141.172045369 4842712.58419657,302300.484950194 4842637.22750659)</t>
+  </si>
+  <si>
+    <t>ROCKBANK CRES S/B N OF STARVIEW DR</t>
+  </si>
+  <si>
+    <t>does not exist</t>
+  </si>
+  <si>
+    <t>wrong desc</t>
+  </si>
+  <si>
+    <t>out of toronto boundary</t>
+  </si>
+  <si>
+    <t>I am super confused by this one</t>
+  </si>
+  <si>
+    <t>wrong: not finch, morningside</t>
   </si>
 </sst>
 </file>
@@ -2316,8 +2768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView topLeftCell="E28" workbookViewId="0">
+      <selection activeCell="P53" sqref="P53:P68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8701,6 +9153,2668 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J98" sqref="J98"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="65.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>15841</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2">
+        <v>14049225</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2">
+        <v>821.38097406071495</v>
+      </c>
+      <c r="H2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>15842</v>
+      </c>
+      <c r="B3" t="s">
+        <v>584</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3">
+        <v>14049225</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3">
+        <v>821.38097406071495</v>
+      </c>
+      <c r="H3" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>26167</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>252</v>
+      </c>
+      <c r="E4">
+        <v>8885835</v>
+      </c>
+      <c r="F4" t="s">
+        <v>253</v>
+      </c>
+      <c r="G4">
+        <v>516.81129859555404</v>
+      </c>
+      <c r="H4" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>22873</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5">
+        <v>914084</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5">
+        <v>474.73744646029797</v>
+      </c>
+      <c r="H5" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>27357</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>349</v>
+      </c>
+      <c r="E6">
+        <v>30038151</v>
+      </c>
+      <c r="F6" t="s">
+        <v>350</v>
+      </c>
+      <c r="G6">
+        <v>430.11296438119598</v>
+      </c>
+      <c r="H6" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>37244</v>
+      </c>
+      <c r="B7" t="s">
+        <v>584</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7">
+        <v>14677598</v>
+      </c>
+      <c r="F7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7">
+        <v>399.00049821458401</v>
+      </c>
+      <c r="H7" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6522</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8">
+        <v>14677598</v>
+      </c>
+      <c r="F8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8">
+        <v>399.00049821458401</v>
+      </c>
+      <c r="H8" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>32081</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>353</v>
+      </c>
+      <c r="E9">
+        <v>30055310</v>
+      </c>
+      <c r="F9" t="s">
+        <v>354</v>
+      </c>
+      <c r="G9">
+        <v>370.99299351475503</v>
+      </c>
+      <c r="H9" t="s">
+        <v>367</v>
+      </c>
+      <c r="I9" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>32082</v>
+      </c>
+      <c r="B10" t="s">
+        <v>584</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>351</v>
+      </c>
+      <c r="E10">
+        <v>30055310</v>
+      </c>
+      <c r="F10" t="s">
+        <v>352</v>
+      </c>
+      <c r="G10">
+        <v>370.99299351475503</v>
+      </c>
+      <c r="H10" t="s">
+        <v>367</v>
+      </c>
+      <c r="I10" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>455</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>293</v>
+      </c>
+      <c r="E11">
+        <v>2967295</v>
+      </c>
+      <c r="F11" t="s">
+        <v>294</v>
+      </c>
+      <c r="G11">
+        <v>315.66848809862398</v>
+      </c>
+      <c r="H11">
+        <v>906898</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>28506</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>295</v>
+      </c>
+      <c r="E12">
+        <v>2967295</v>
+      </c>
+      <c r="F12" t="s">
+        <v>296</v>
+      </c>
+      <c r="G12">
+        <v>315.66848809862398</v>
+      </c>
+      <c r="H12">
+        <v>906898</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>23587</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13">
+        <v>443573</v>
+      </c>
+      <c r="F13" t="s">
+        <v>95</v>
+      </c>
+      <c r="G13">
+        <v>311.24049275696001</v>
+      </c>
+      <c r="H13" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>23553</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14">
+        <v>443573</v>
+      </c>
+      <c r="F14" t="s">
+        <v>93</v>
+      </c>
+      <c r="G14">
+        <v>311.24049275696001</v>
+      </c>
+      <c r="H14" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>3512</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>359</v>
+      </c>
+      <c r="E15">
+        <v>14308141</v>
+      </c>
+      <c r="F15" t="s">
+        <v>360</v>
+      </c>
+      <c r="G15">
+        <v>298.53323658976302</v>
+      </c>
+      <c r="H15" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>3243</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>331</v>
+      </c>
+      <c r="E16">
+        <v>14668493</v>
+      </c>
+      <c r="F16" t="s">
+        <v>332</v>
+      </c>
+      <c r="G16">
+        <v>296.41020978882301</v>
+      </c>
+      <c r="H16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>30546</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>655</v>
+      </c>
+      <c r="E17">
+        <v>20059734</v>
+      </c>
+      <c r="F17" t="s">
+        <v>656</v>
+      </c>
+      <c r="G17">
+        <v>283.84933884210602</v>
+      </c>
+      <c r="H17" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16228</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>657</v>
+      </c>
+      <c r="E18">
+        <v>11485087</v>
+      </c>
+      <c r="F18" t="s">
+        <v>658</v>
+      </c>
+      <c r="G18">
+        <v>273.05210342203998</v>
+      </c>
+      <c r="H18" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>16229</v>
+      </c>
+      <c r="B19" t="s">
+        <v>584</v>
+      </c>
+      <c r="C19" t="s">
+        <v>577</v>
+      </c>
+      <c r="D19" t="s">
+        <v>659</v>
+      </c>
+      <c r="E19">
+        <v>11485087</v>
+      </c>
+      <c r="F19" t="s">
+        <v>660</v>
+      </c>
+      <c r="G19">
+        <v>273.05210342203998</v>
+      </c>
+      <c r="H19" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>16510</v>
+      </c>
+      <c r="B20" t="s">
+        <v>584</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20">
+        <v>13971133</v>
+      </c>
+      <c r="F20" t="s">
+        <v>131</v>
+      </c>
+      <c r="G20">
+        <v>267.10480645476599</v>
+      </c>
+      <c r="H20" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>16509</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
+        <v>128</v>
+      </c>
+      <c r="E21">
+        <v>13971133</v>
+      </c>
+      <c r="F21" t="s">
+        <v>129</v>
+      </c>
+      <c r="G21">
+        <v>267.10480645476599</v>
+      </c>
+      <c r="H21" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>24126</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" t="s">
+        <v>160</v>
+      </c>
+      <c r="E22">
+        <v>30029305</v>
+      </c>
+      <c r="F22" t="s">
+        <v>161</v>
+      </c>
+      <c r="G22">
+        <v>257.86086466498699</v>
+      </c>
+      <c r="H22">
+        <v>30029306</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>3823</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s">
+        <v>661</v>
+      </c>
+      <c r="E23">
+        <v>30021327</v>
+      </c>
+      <c r="F23" t="s">
+        <v>662</v>
+      </c>
+      <c r="G23">
+        <v>243.91482263914699</v>
+      </c>
+      <c r="H23">
+        <v>30037208</v>
+      </c>
+      <c r="I23" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>34316</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>663</v>
+      </c>
+      <c r="E24">
+        <v>112499</v>
+      </c>
+      <c r="F24" t="s">
+        <v>664</v>
+      </c>
+      <c r="G24">
+        <v>233.037996309188</v>
+      </c>
+      <c r="H24">
+        <v>30012958</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>34317</v>
+      </c>
+      <c r="B25" t="s">
+        <v>584</v>
+      </c>
+      <c r="C25" t="s">
+        <v>577</v>
+      </c>
+      <c r="D25" t="s">
+        <v>665</v>
+      </c>
+      <c r="E25">
+        <v>112499</v>
+      </c>
+      <c r="F25" t="s">
+        <v>666</v>
+      </c>
+      <c r="G25">
+        <v>233.037996309188</v>
+      </c>
+      <c r="H25">
+        <v>30012958</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>26613</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" t="s">
+        <v>355</v>
+      </c>
+      <c r="E26">
+        <v>30007958</v>
+      </c>
+      <c r="F26" t="s">
+        <v>356</v>
+      </c>
+      <c r="G26">
+        <v>230.74923735018101</v>
+      </c>
+      <c r="H26" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26614</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" t="s">
+        <v>357</v>
+      </c>
+      <c r="E27">
+        <v>30007958</v>
+      </c>
+      <c r="F27" t="s">
+        <v>358</v>
+      </c>
+      <c r="G27">
+        <v>230.74923735018101</v>
+      </c>
+      <c r="H27" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>26452</v>
+      </c>
+      <c r="B28" t="s">
+        <v>584</v>
+      </c>
+      <c r="C28" t="s">
+        <v>577</v>
+      </c>
+      <c r="D28" t="s">
+        <v>378</v>
+      </c>
+      <c r="E28">
+        <v>444811</v>
+      </c>
+      <c r="F28" t="s">
+        <v>379</v>
+      </c>
+      <c r="G28">
+        <v>221.628515328925</v>
+      </c>
+      <c r="H28" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>30586</v>
+      </c>
+      <c r="B29" t="s">
+        <v>584</v>
+      </c>
+      <c r="C29" t="s">
+        <v>577</v>
+      </c>
+      <c r="D29" t="s">
+        <v>283</v>
+      </c>
+      <c r="E29">
+        <v>443179</v>
+      </c>
+      <c r="F29" t="s">
+        <v>284</v>
+      </c>
+      <c r="G29">
+        <v>219.176009918772</v>
+      </c>
+      <c r="H29" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>34009</v>
+      </c>
+      <c r="B30" t="s">
+        <v>584</v>
+      </c>
+      <c r="C30" t="s">
+        <v>577</v>
+      </c>
+      <c r="D30" t="s">
+        <v>363</v>
+      </c>
+      <c r="E30">
+        <v>9344363</v>
+      </c>
+      <c r="F30" t="s">
+        <v>364</v>
+      </c>
+      <c r="G30">
+        <v>217.757391033673</v>
+      </c>
+      <c r="H30">
+        <v>30073636</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>34008</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" t="s">
+        <v>365</v>
+      </c>
+      <c r="E31">
+        <v>9344363</v>
+      </c>
+      <c r="F31" t="s">
+        <v>366</v>
+      </c>
+      <c r="G31">
+        <v>217.757391033673</v>
+      </c>
+      <c r="H31">
+        <v>30073636</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>29430</v>
+      </c>
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" t="s">
+        <v>264</v>
+      </c>
+      <c r="E32">
+        <v>649</v>
+      </c>
+      <c r="F32" t="s">
+        <v>667</v>
+      </c>
+      <c r="G32">
+        <v>213.145067031118</v>
+      </c>
+      <c r="H32" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>29970</v>
+      </c>
+      <c r="B33" t="s">
+        <v>584</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33">
+        <v>4124720</v>
+      </c>
+      <c r="F33" t="s">
+        <v>44</v>
+      </c>
+      <c r="G33">
+        <v>205.10786986894001</v>
+      </c>
+      <c r="H33">
+        <v>104477</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>30618</v>
+      </c>
+      <c r="B34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>668</v>
+      </c>
+      <c r="E34">
+        <v>30083324</v>
+      </c>
+      <c r="F34" t="s">
+        <v>669</v>
+      </c>
+      <c r="G34">
+        <v>192.65067786979699</v>
+      </c>
+      <c r="H34" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>22857</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" t="s">
+        <v>670</v>
+      </c>
+      <c r="E35">
+        <v>20040308</v>
+      </c>
+      <c r="F35" t="s">
+        <v>671</v>
+      </c>
+      <c r="G35">
+        <v>185.23620189718</v>
+      </c>
+      <c r="H35" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>12771</v>
+      </c>
+      <c r="B36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" t="s">
+        <v>345</v>
+      </c>
+      <c r="E36">
+        <v>30029984</v>
+      </c>
+      <c r="F36" t="s">
+        <v>346</v>
+      </c>
+      <c r="G36">
+        <v>180.578387777503</v>
+      </c>
+      <c r="H36" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>12772</v>
+      </c>
+      <c r="B37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" t="s">
+        <v>347</v>
+      </c>
+      <c r="E37">
+        <v>30029984</v>
+      </c>
+      <c r="F37" t="s">
+        <v>348</v>
+      </c>
+      <c r="G37">
+        <v>180.578387777503</v>
+      </c>
+      <c r="H37" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1295</v>
+      </c>
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" t="s">
+        <v>672</v>
+      </c>
+      <c r="E38">
+        <v>30006420</v>
+      </c>
+      <c r="F38" t="s">
+        <v>673</v>
+      </c>
+      <c r="G38">
+        <v>173.212809581865</v>
+      </c>
+      <c r="H38" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>26231</v>
+      </c>
+      <c r="B39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" t="s">
+        <v>577</v>
+      </c>
+      <c r="D39" t="s">
+        <v>674</v>
+      </c>
+      <c r="E39">
+        <v>30006223</v>
+      </c>
+      <c r="F39" t="s">
+        <v>675</v>
+      </c>
+      <c r="G39">
+        <v>165.70834606353199</v>
+      </c>
+      <c r="H39" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>26230</v>
+      </c>
+      <c r="B40" t="s">
+        <v>584</v>
+      </c>
+      <c r="C40" t="s">
+        <v>577</v>
+      </c>
+      <c r="D40" t="s">
+        <v>676</v>
+      </c>
+      <c r="E40">
+        <v>30006223</v>
+      </c>
+      <c r="F40" t="s">
+        <v>677</v>
+      </c>
+      <c r="G40">
+        <v>165.70834606353199</v>
+      </c>
+      <c r="H40" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>35436</v>
+      </c>
+      <c r="B41" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>678</v>
+      </c>
+      <c r="E41">
+        <v>30011000</v>
+      </c>
+      <c r="F41" t="s">
+        <v>679</v>
+      </c>
+      <c r="G41">
+        <v>156.17312276456801</v>
+      </c>
+      <c r="H41" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>30650</v>
+      </c>
+      <c r="B42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>680</v>
+      </c>
+      <c r="E42">
+        <v>30077643</v>
+      </c>
+      <c r="F42" t="s">
+        <v>681</v>
+      </c>
+      <c r="G42">
+        <v>152.26763925022601</v>
+      </c>
+      <c r="H42" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>30649</v>
+      </c>
+      <c r="B43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>682</v>
+      </c>
+      <c r="E43">
+        <v>30077643</v>
+      </c>
+      <c r="F43" t="s">
+        <v>683</v>
+      </c>
+      <c r="G43">
+        <v>152.26763925022601</v>
+      </c>
+      <c r="H43" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>1189</v>
+      </c>
+      <c r="B44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" t="s">
+        <v>684</v>
+      </c>
+      <c r="E44">
+        <v>30076029</v>
+      </c>
+      <c r="F44" t="s">
+        <v>685</v>
+      </c>
+      <c r="G44">
+        <v>151.91418678343999</v>
+      </c>
+      <c r="H44" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>32994</v>
+      </c>
+      <c r="B45" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" t="s">
+        <v>686</v>
+      </c>
+      <c r="E45">
+        <v>30059997</v>
+      </c>
+      <c r="F45" t="s">
+        <v>687</v>
+      </c>
+      <c r="G45">
+        <v>146.37831805536101</v>
+      </c>
+      <c r="H45" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>32993</v>
+      </c>
+      <c r="B46" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" t="s">
+        <v>688</v>
+      </c>
+      <c r="E46">
+        <v>30059997</v>
+      </c>
+      <c r="F46" t="s">
+        <v>689</v>
+      </c>
+      <c r="G46">
+        <v>146.37831805536101</v>
+      </c>
+      <c r="H46" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>27776</v>
+      </c>
+      <c r="B47" t="s">
+        <v>584</v>
+      </c>
+      <c r="C47" t="s">
+        <v>577</v>
+      </c>
+      <c r="D47" t="s">
+        <v>690</v>
+      </c>
+      <c r="E47">
+        <v>30070013</v>
+      </c>
+      <c r="F47" t="s">
+        <v>691</v>
+      </c>
+      <c r="G47">
+        <v>145.44192013306801</v>
+      </c>
+      <c r="H47" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>27895</v>
+      </c>
+      <c r="B48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" t="s">
+        <v>692</v>
+      </c>
+      <c r="E48">
+        <v>10459142</v>
+      </c>
+      <c r="F48" t="s">
+        <v>693</v>
+      </c>
+      <c r="G48">
+        <v>144.46626315264601</v>
+      </c>
+      <c r="H48" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>32188</v>
+      </c>
+      <c r="B49" t="s">
+        <v>584</v>
+      </c>
+      <c r="C49" t="s">
+        <v>577</v>
+      </c>
+      <c r="D49" t="s">
+        <v>694</v>
+      </c>
+      <c r="E49">
+        <v>20230426</v>
+      </c>
+      <c r="F49" t="s">
+        <v>695</v>
+      </c>
+      <c r="G49">
+        <v>142.477545845348</v>
+      </c>
+      <c r="H49" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>1192</v>
+      </c>
+      <c r="B50" t="s">
+        <v>584</v>
+      </c>
+      <c r="C50" t="s">
+        <v>577</v>
+      </c>
+      <c r="D50" t="s">
+        <v>696</v>
+      </c>
+      <c r="E50">
+        <v>30067121</v>
+      </c>
+      <c r="F50" t="s">
+        <v>697</v>
+      </c>
+      <c r="G50">
+        <v>135.86962933852101</v>
+      </c>
+      <c r="H50" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>16702</v>
+      </c>
+      <c r="B51" t="s">
+        <v>584</v>
+      </c>
+      <c r="C51" t="s">
+        <v>577</v>
+      </c>
+      <c r="D51" t="s">
+        <v>698</v>
+      </c>
+      <c r="E51">
+        <v>14063435</v>
+      </c>
+      <c r="F51" t="s">
+        <v>699</v>
+      </c>
+      <c r="G51">
+        <v>135.41035623490799</v>
+      </c>
+      <c r="H51" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>16672</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" t="s">
+        <v>577</v>
+      </c>
+      <c r="D52" t="s">
+        <v>700</v>
+      </c>
+      <c r="E52">
+        <v>14063435</v>
+      </c>
+      <c r="F52" t="s">
+        <v>701</v>
+      </c>
+      <c r="G52">
+        <v>135.41035623490799</v>
+      </c>
+      <c r="H52" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>1980</v>
+      </c>
+      <c r="B53" t="s">
+        <v>584</v>
+      </c>
+      <c r="C53" t="s">
+        <v>577</v>
+      </c>
+      <c r="D53" t="s">
+        <v>702</v>
+      </c>
+      <c r="E53">
+        <v>440202</v>
+      </c>
+      <c r="F53" t="s">
+        <v>703</v>
+      </c>
+      <c r="G53">
+        <v>134.937769301011</v>
+      </c>
+      <c r="H53">
+        <v>20140757</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>30384</v>
+      </c>
+      <c r="B54" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" t="s">
+        <v>704</v>
+      </c>
+      <c r="E54">
+        <v>30029963</v>
+      </c>
+      <c r="F54" t="s">
+        <v>705</v>
+      </c>
+      <c r="G54">
+        <v>133.352091425146</v>
+      </c>
+      <c r="H54" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>12628</v>
+      </c>
+      <c r="B55" t="s">
+        <v>15</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>706</v>
+      </c>
+      <c r="E55">
+        <v>20042254</v>
+      </c>
+      <c r="F55" t="s">
+        <v>707</v>
+      </c>
+      <c r="G55">
+        <v>131.84880497173799</v>
+      </c>
+      <c r="H55" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>12627</v>
+      </c>
+      <c r="B56" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>708</v>
+      </c>
+      <c r="E56">
+        <v>20042254</v>
+      </c>
+      <c r="F56" t="s">
+        <v>709</v>
+      </c>
+      <c r="G56">
+        <v>131.84880497173799</v>
+      </c>
+      <c r="H56" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>34174</v>
+      </c>
+      <c r="B57" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>710</v>
+      </c>
+      <c r="E57">
+        <v>20235444</v>
+      </c>
+      <c r="F57" t="s">
+        <v>711</v>
+      </c>
+      <c r="G57">
+        <v>130.807275711073</v>
+      </c>
+      <c r="H57" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>23816</v>
+      </c>
+      <c r="B58" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" t="s">
+        <v>712</v>
+      </c>
+      <c r="E58">
+        <v>20235444</v>
+      </c>
+      <c r="F58" t="s">
+        <v>713</v>
+      </c>
+      <c r="G58">
+        <v>130.807275711073</v>
+      </c>
+      <c r="H58" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>35264</v>
+      </c>
+      <c r="B59" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
+        <v>714</v>
+      </c>
+      <c r="E59">
+        <v>30070003</v>
+      </c>
+      <c r="F59" t="s">
+        <v>715</v>
+      </c>
+      <c r="G59">
+        <v>128.185446824797</v>
+      </c>
+      <c r="H59" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>15114</v>
+      </c>
+      <c r="B60" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" t="s">
+        <v>716</v>
+      </c>
+      <c r="E60">
+        <v>30040145</v>
+      </c>
+      <c r="F60" t="s">
+        <v>717</v>
+      </c>
+      <c r="G60">
+        <v>125.219281559001</v>
+      </c>
+      <c r="H60" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>15113</v>
+      </c>
+      <c r="B61" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" t="s">
+        <v>718</v>
+      </c>
+      <c r="E61">
+        <v>30040145</v>
+      </c>
+      <c r="F61" t="s">
+        <v>719</v>
+      </c>
+      <c r="G61">
+        <v>125.219281559001</v>
+      </c>
+      <c r="H61" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>31694</v>
+      </c>
+      <c r="B62" t="s">
+        <v>15</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
+        <v>720</v>
+      </c>
+      <c r="E62">
+        <v>30062735</v>
+      </c>
+      <c r="F62" t="s">
+        <v>721</v>
+      </c>
+      <c r="G62">
+        <v>123.327126900615</v>
+      </c>
+      <c r="H62" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>31695</v>
+      </c>
+      <c r="B63" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
+        <v>722</v>
+      </c>
+      <c r="E63">
+        <v>30062735</v>
+      </c>
+      <c r="F63" t="s">
+        <v>723</v>
+      </c>
+      <c r="G63">
+        <v>123.327126900615</v>
+      </c>
+      <c r="H63" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>6493</v>
+      </c>
+      <c r="B64" t="s">
+        <v>584</v>
+      </c>
+      <c r="C64" t="s">
+        <v>577</v>
+      </c>
+      <c r="D64" t="s">
+        <v>724</v>
+      </c>
+      <c r="E64">
+        <v>907234</v>
+      </c>
+      <c r="F64" t="s">
+        <v>725</v>
+      </c>
+      <c r="G64">
+        <v>121.700472000224</v>
+      </c>
+      <c r="H64" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>6542</v>
+      </c>
+      <c r="B65" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65" t="s">
+        <v>577</v>
+      </c>
+      <c r="D65" t="s">
+        <v>726</v>
+      </c>
+      <c r="E65">
+        <v>907234</v>
+      </c>
+      <c r="F65" t="s">
+        <v>727</v>
+      </c>
+      <c r="G65">
+        <v>121.700472000224</v>
+      </c>
+      <c r="H65" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>25357</v>
+      </c>
+      <c r="B66" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1</v>
+      </c>
+      <c r="D66" t="s">
+        <v>728</v>
+      </c>
+      <c r="E66">
+        <v>441406</v>
+      </c>
+      <c r="F66" t="s">
+        <v>729</v>
+      </c>
+      <c r="G66">
+        <v>120.10239053847199</v>
+      </c>
+      <c r="H66">
+        <v>20041330</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>25360</v>
+      </c>
+      <c r="B67" t="s">
+        <v>2</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1</v>
+      </c>
+      <c r="D67" t="s">
+        <v>730</v>
+      </c>
+      <c r="E67">
+        <v>441406</v>
+      </c>
+      <c r="F67" t="s">
+        <v>731</v>
+      </c>
+      <c r="G67">
+        <v>120.10239053847199</v>
+      </c>
+      <c r="H67">
+        <v>20041330</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>1979</v>
+      </c>
+      <c r="B68" t="s">
+        <v>11</v>
+      </c>
+      <c r="C68" t="s">
+        <v>10</v>
+      </c>
+      <c r="D68" t="s">
+        <v>732</v>
+      </c>
+      <c r="E68">
+        <v>20140757</v>
+      </c>
+      <c r="F68" t="s">
+        <v>733</v>
+      </c>
+      <c r="G68">
+        <v>119.30927534065</v>
+      </c>
+      <c r="H68" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>3285</v>
+      </c>
+      <c r="B69" t="s">
+        <v>11</v>
+      </c>
+      <c r="C69" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69" t="s">
+        <v>734</v>
+      </c>
+      <c r="E69">
+        <v>30011526</v>
+      </c>
+      <c r="F69" t="s">
+        <v>735</v>
+      </c>
+      <c r="G69">
+        <v>118.49646406475</v>
+      </c>
+      <c r="H69">
+        <v>30011544</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>23130</v>
+      </c>
+      <c r="B70" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70" t="s">
+        <v>10</v>
+      </c>
+      <c r="D70" t="s">
+        <v>736</v>
+      </c>
+      <c r="E70">
+        <v>913167</v>
+      </c>
+      <c r="F70" t="s">
+        <v>737</v>
+      </c>
+      <c r="G70">
+        <v>117.356502583984</v>
+      </c>
+      <c r="H70" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>14567</v>
+      </c>
+      <c r="B71" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71" t="s">
+        <v>738</v>
+      </c>
+      <c r="E71">
+        <v>30003826</v>
+      </c>
+      <c r="F71" t="s">
+        <v>739</v>
+      </c>
+      <c r="G71">
+        <v>117.186430799831</v>
+      </c>
+      <c r="H71" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>14566</v>
+      </c>
+      <c r="B72" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72" t="s">
+        <v>14</v>
+      </c>
+      <c r="D72" t="s">
+        <v>740</v>
+      </c>
+      <c r="E72">
+        <v>30003826</v>
+      </c>
+      <c r="F72" t="s">
+        <v>741</v>
+      </c>
+      <c r="G72">
+        <v>117.186430799831</v>
+      </c>
+      <c r="H72" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>27943</v>
+      </c>
+      <c r="B73" t="s">
+        <v>11</v>
+      </c>
+      <c r="C73" t="s">
+        <v>10</v>
+      </c>
+      <c r="D73" t="s">
+        <v>742</v>
+      </c>
+      <c r="E73">
+        <v>30074690</v>
+      </c>
+      <c r="F73" t="s">
+        <v>743</v>
+      </c>
+      <c r="G73">
+        <v>115.073515298443</v>
+      </c>
+      <c r="H73" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>34486</v>
+      </c>
+      <c r="B74" t="s">
+        <v>584</v>
+      </c>
+      <c r="C74" t="s">
+        <v>577</v>
+      </c>
+      <c r="D74" t="s">
+        <v>744</v>
+      </c>
+      <c r="E74">
+        <v>7731502</v>
+      </c>
+      <c r="F74" t="s">
+        <v>745</v>
+      </c>
+      <c r="G74">
+        <v>114.664688200535</v>
+      </c>
+      <c r="H74" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>16744</v>
+      </c>
+      <c r="B75" t="s">
+        <v>11</v>
+      </c>
+      <c r="C75" t="s">
+        <v>577</v>
+      </c>
+      <c r="D75" t="s">
+        <v>746</v>
+      </c>
+      <c r="E75">
+        <v>14063800</v>
+      </c>
+      <c r="F75" t="s">
+        <v>747</v>
+      </c>
+      <c r="G75">
+        <v>112.86873583900601</v>
+      </c>
+      <c r="H75" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>16746</v>
+      </c>
+      <c r="B76" t="s">
+        <v>584</v>
+      </c>
+      <c r="C76" t="s">
+        <v>577</v>
+      </c>
+      <c r="D76" t="s">
+        <v>748</v>
+      </c>
+      <c r="E76">
+        <v>14063800</v>
+      </c>
+      <c r="F76" t="s">
+        <v>749</v>
+      </c>
+      <c r="G76">
+        <v>112.86873583900601</v>
+      </c>
+      <c r="H76" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>30740</v>
+      </c>
+      <c r="B77" t="s">
+        <v>2</v>
+      </c>
+      <c r="C77" t="s">
+        <v>14</v>
+      </c>
+      <c r="D77" t="s">
+        <v>750</v>
+      </c>
+      <c r="E77">
+        <v>3093329</v>
+      </c>
+      <c r="F77" t="s">
+        <v>751</v>
+      </c>
+      <c r="G77">
+        <v>108.129894978175</v>
+      </c>
+      <c r="H77" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>30739</v>
+      </c>
+      <c r="B78" t="s">
+        <v>15</v>
+      </c>
+      <c r="C78" t="s">
+        <v>14</v>
+      </c>
+      <c r="D78" t="s">
+        <v>752</v>
+      </c>
+      <c r="E78">
+        <v>3093329</v>
+      </c>
+      <c r="F78" t="s">
+        <v>753</v>
+      </c>
+      <c r="G78">
+        <v>108.129894978175</v>
+      </c>
+      <c r="H78" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>3278</v>
+      </c>
+      <c r="B79" t="s">
+        <v>11</v>
+      </c>
+      <c r="C79" t="s">
+        <v>10</v>
+      </c>
+      <c r="D79" t="s">
+        <v>754</v>
+      </c>
+      <c r="E79">
+        <v>30037426</v>
+      </c>
+      <c r="F79" t="s">
+        <v>755</v>
+      </c>
+      <c r="G79">
+        <v>107.912614542488</v>
+      </c>
+      <c r="H79" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>33307</v>
+      </c>
+      <c r="B80" t="s">
+        <v>11</v>
+      </c>
+      <c r="C80" t="s">
+        <v>577</v>
+      </c>
+      <c r="D80" t="s">
+        <v>756</v>
+      </c>
+      <c r="E80">
+        <v>30004153</v>
+      </c>
+      <c r="F80" t="s">
+        <v>757</v>
+      </c>
+      <c r="G80">
+        <v>104.93169397030999</v>
+      </c>
+      <c r="H80" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>5</v>
+      </c>
+      <c r="B81" t="s">
+        <v>584</v>
+      </c>
+      <c r="C81" t="s">
+        <v>577</v>
+      </c>
+      <c r="D81" t="s">
+        <v>758</v>
+      </c>
+      <c r="E81">
+        <v>30004153</v>
+      </c>
+      <c r="F81" t="s">
+        <v>759</v>
+      </c>
+      <c r="G81">
+        <v>104.93169397030999</v>
+      </c>
+      <c r="H81" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>1458</v>
+      </c>
+      <c r="B82" t="s">
+        <v>11</v>
+      </c>
+      <c r="C82" t="s">
+        <v>10</v>
+      </c>
+      <c r="D82" t="s">
+        <v>760</v>
+      </c>
+      <c r="E82">
+        <v>20362226</v>
+      </c>
+      <c r="F82" t="s">
+        <v>761</v>
+      </c>
+      <c r="G82">
+        <v>103.15055400767901</v>
+      </c>
+      <c r="H82" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>1413</v>
+      </c>
+      <c r="B83" t="s">
+        <v>584</v>
+      </c>
+      <c r="C83" t="s">
+        <v>577</v>
+      </c>
+      <c r="D83" t="s">
+        <v>762</v>
+      </c>
+      <c r="E83">
+        <v>20362226</v>
+      </c>
+      <c r="F83" t="s">
+        <v>763</v>
+      </c>
+      <c r="G83">
+        <v>103.15055400767901</v>
+      </c>
+      <c r="H83" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>3731</v>
+      </c>
+      <c r="B84" t="s">
+        <v>2</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1</v>
+      </c>
+      <c r="D84" t="s">
+        <v>764</v>
+      </c>
+      <c r="E84">
+        <v>20164338</v>
+      </c>
+      <c r="F84" t="s">
+        <v>765</v>
+      </c>
+      <c r="G84">
+        <v>102.247209403483</v>
+      </c>
+      <c r="H84" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>23414</v>
+      </c>
+      <c r="B85" t="s">
+        <v>2</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1</v>
+      </c>
+      <c r="D85" t="s">
+        <v>766</v>
+      </c>
+      <c r="E85">
+        <v>30017340</v>
+      </c>
+      <c r="F85" t="s">
+        <v>767</v>
+      </c>
+      <c r="G85">
+        <v>102.103843517315</v>
+      </c>
+      <c r="H85" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>33160</v>
+      </c>
+      <c r="B86" t="s">
+        <v>2</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1</v>
+      </c>
+      <c r="D86" t="s">
+        <v>768</v>
+      </c>
+      <c r="E86">
+        <v>14252787</v>
+      </c>
+      <c r="F86" t="s">
+        <v>769</v>
+      </c>
+      <c r="G86">
+        <v>101.38385873968301</v>
+      </c>
+      <c r="H86">
+        <v>14307786</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>33159</v>
+      </c>
+      <c r="B87" t="s">
+        <v>15</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1</v>
+      </c>
+      <c r="D87" t="s">
+        <v>770</v>
+      </c>
+      <c r="E87">
+        <v>14252787</v>
+      </c>
+      <c r="F87" t="s">
+        <v>771</v>
+      </c>
+      <c r="G87">
+        <v>101.38385873968301</v>
+      </c>
+      <c r="H87">
+        <v>14307786</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>35538</v>
+      </c>
+      <c r="B88" t="s">
+        <v>584</v>
+      </c>
+      <c r="C88" t="s">
+        <v>577</v>
+      </c>
+      <c r="D88" t="s">
+        <v>772</v>
+      </c>
+      <c r="E88">
+        <v>30039431</v>
+      </c>
+      <c r="F88" t="s">
+        <v>773</v>
+      </c>
+      <c r="G88">
+        <v>101.316876322643</v>
+      </c>
+      <c r="H88" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>35537</v>
+      </c>
+      <c r="B89" t="s">
+        <v>11</v>
+      </c>
+      <c r="C89" t="s">
+        <v>10</v>
+      </c>
+      <c r="D89" t="s">
+        <v>774</v>
+      </c>
+      <c r="E89">
+        <v>30039431</v>
+      </c>
+      <c r="F89" t="s">
+        <v>775</v>
+      </c>
+      <c r="G89">
+        <v>101.316876322643</v>
+      </c>
+      <c r="H89" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>23118</v>
+      </c>
+      <c r="B90" t="s">
+        <v>2</v>
+      </c>
+      <c r="C90" t="s">
+        <v>1</v>
+      </c>
+      <c r="D90" t="s">
+        <v>776</v>
+      </c>
+      <c r="E90">
+        <v>30064879</v>
+      </c>
+      <c r="F90" t="s">
+        <v>777</v>
+      </c>
+      <c r="G90">
+        <v>99.922255445578102</v>
+      </c>
+      <c r="H90" t="s">
+        <v>367</v>
+      </c>
+      <c r="I90" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>2580</v>
+      </c>
+      <c r="B91" t="s">
+        <v>15</v>
+      </c>
+      <c r="C91" t="s">
+        <v>1</v>
+      </c>
+      <c r="D91" t="s">
+        <v>778</v>
+      </c>
+      <c r="E91">
+        <v>30064879</v>
+      </c>
+      <c r="F91" t="s">
+        <v>779</v>
+      </c>
+      <c r="G91">
+        <v>99.922255445578102</v>
+      </c>
+      <c r="H91" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>28922</v>
+      </c>
+      <c r="B92" t="s">
+        <v>11</v>
+      </c>
+      <c r="C92" t="s">
+        <v>10</v>
+      </c>
+      <c r="D92" t="s">
+        <v>780</v>
+      </c>
+      <c r="E92">
+        <v>442957</v>
+      </c>
+      <c r="F92" t="s">
+        <v>781</v>
+      </c>
+      <c r="G92">
+        <v>98.028419307202398</v>
+      </c>
+      <c r="H92">
+        <v>30085272</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>28921</v>
+      </c>
+      <c r="B93" t="s">
+        <v>584</v>
+      </c>
+      <c r="C93" t="s">
+        <v>577</v>
+      </c>
+      <c r="D93" t="s">
+        <v>782</v>
+      </c>
+      <c r="E93">
+        <v>442957</v>
+      </c>
+      <c r="F93" t="s">
+        <v>783</v>
+      </c>
+      <c r="G93">
+        <v>98.028419307202398</v>
+      </c>
+      <c r="H93">
+        <v>30085273</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>405</v>
+      </c>
+      <c r="B94" t="s">
+        <v>15</v>
+      </c>
+      <c r="C94" t="s">
+        <v>14</v>
+      </c>
+      <c r="D94" t="s">
+        <v>784</v>
+      </c>
+      <c r="E94">
+        <v>30034345</v>
+      </c>
+      <c r="F94" t="s">
+        <v>785</v>
+      </c>
+      <c r="G94">
+        <v>92.421179019919094</v>
+      </c>
+      <c r="H94" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>397</v>
+      </c>
+      <c r="B95" t="s">
+        <v>2</v>
+      </c>
+      <c r="C95" t="s">
+        <v>14</v>
+      </c>
+      <c r="D95" t="s">
+        <v>786</v>
+      </c>
+      <c r="E95">
+        <v>30034345</v>
+      </c>
+      <c r="F95" t="s">
+        <v>787</v>
+      </c>
+      <c r="G95">
+        <v>92.421179019919094</v>
+      </c>
+      <c r="H95" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>33001</v>
+      </c>
+      <c r="B96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C96" t="s">
+        <v>1</v>
+      </c>
+      <c r="D96" t="s">
+        <v>788</v>
+      </c>
+      <c r="E96">
+        <v>20050211</v>
+      </c>
+      <c r="F96" t="s">
+        <v>789</v>
+      </c>
+      <c r="G96">
+        <v>91.134487364898007</v>
+      </c>
+      <c r="H96" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>33002</v>
+      </c>
+      <c r="B97" t="s">
+        <v>2</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1</v>
+      </c>
+      <c r="D97" t="s">
+        <v>790</v>
+      </c>
+      <c r="E97">
+        <v>20050211</v>
+      </c>
+      <c r="F97" t="s">
+        <v>791</v>
+      </c>
+      <c r="G97">
+        <v>91.134487364898007</v>
+      </c>
+      <c r="H97" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>29175</v>
+      </c>
+      <c r="B98" t="s">
+        <v>2</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1</v>
+      </c>
+      <c r="D98" t="s">
+        <v>792</v>
+      </c>
+      <c r="E98">
+        <v>30035854</v>
+      </c>
+      <c r="F98" t="s">
+        <v>793</v>
+      </c>
+      <c r="G98">
+        <v>86.473466839192696</v>
+      </c>
+      <c r="H98" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>29174</v>
+      </c>
+      <c r="B99" t="s">
+        <v>15</v>
+      </c>
+      <c r="C99" t="s">
+        <v>14</v>
+      </c>
+      <c r="D99" t="s">
+        <v>794</v>
+      </c>
+      <c r="E99">
+        <v>30035854</v>
+      </c>
+      <c r="F99" t="s">
+        <v>795</v>
+      </c>
+      <c r="G99">
+        <v>86.473466839192696</v>
+      </c>
+      <c r="H99" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>22250</v>
+      </c>
+      <c r="B100" t="s">
+        <v>15</v>
+      </c>
+      <c r="C100" t="s">
+        <v>14</v>
+      </c>
+      <c r="D100" t="s">
+        <v>796</v>
+      </c>
+      <c r="E100">
+        <v>10486741</v>
+      </c>
+      <c r="F100" t="s">
+        <v>797</v>
+      </c>
+      <c r="G100">
+        <v>85.0623305445543</v>
+      </c>
+      <c r="H100">
+        <v>10487714</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>22251</v>
+      </c>
+      <c r="B101" t="s">
+        <v>2</v>
+      </c>
+      <c r="C101" t="s">
+        <v>1</v>
+      </c>
+      <c r="D101" t="s">
+        <v>798</v>
+      </c>
+      <c r="E101">
+        <v>10486741</v>
+      </c>
+      <c r="F101" t="s">
+        <v>799</v>
+      </c>
+      <c r="G101">
+        <v>85.0623305445543</v>
+      </c>
+      <c r="H101">
+        <v>10487714</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9738,7 +12852,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
@@ -10196,7 +13310,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>

</xml_diff>